<commit_message>
allow 1-D plot cuts for real&sim
</commit_message>
<xml_diff>
--- a/in/2cam_sweep.xlsx
+++ b/in/2cam_sweep.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="994" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sim" sheetId="1" state="visible" r:id="rId2"/>
@@ -144,7 +144,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A59" authorId="0">
+    <comment ref="A60" authorId="0">
       <text>
         <r>
           <rPr>
@@ -162,7 +162,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A64" authorId="0">
+    <comment ref="A65" authorId="0">
       <text>
         <r>
           <rPr>
@@ -320,7 +320,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="134">
   <si>
     <t>Sim</t>
   </si>
@@ -518,6 +518,9 @@
   </si>
   <si>
     <t>OptimMaxiter</t>
+  </si>
+  <si>
+    <t>minflux</t>
   </si>
   <si>
     <t>maxIter</t>
@@ -1357,12 +1360,12 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H73"/>
+  <dimension ref="A1:H74"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D48" activeCellId="0" sqref="D48"/>
+      <selection pane="bottomLeft" activeCell="E55" activeCellId="0" sqref="E55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1723,7 +1726,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
         <v>48</v>
       </c>
@@ -1875,7 +1878,7 @@
       <c r="G47" s="0"/>
       <c r="H47" s="0"/>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="31" t="s">
         <v>60</v>
       </c>
@@ -1940,7 +1943,7 @@
       </c>
       <c r="F53" s="13"/>
     </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="4" t="s">
         <v>65</v>
       </c>
@@ -1952,18 +1955,22 @@
       </c>
       <c r="F54" s="13"/>
     </row>
-    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="38"/>
-      <c r="B55" s="39"/>
-      <c r="C55" s="39"/>
-    </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="4" t="s">
+    <row r="55" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="B56" s="0"/>
-      <c r="C56" s="0"/>
-      <c r="F56" s="40"/>
+      <c r="B55" s="0"/>
+      <c r="C55" s="0"/>
+      <c r="D55" s="5"/>
+      <c r="E55" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F55" s="13"/>
+    </row>
+    <row r="56" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="38"/>
+      <c r="B56" s="39"/>
+      <c r="C56" s="39"/>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="4" t="s">
@@ -1971,7 +1978,7 @@
       </c>
       <c r="B57" s="0"/>
       <c r="C57" s="0"/>
-      <c r="F57" s="41"/>
+      <c r="F57" s="40"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="4" t="s">
@@ -1979,7 +1986,7 @@
       </c>
       <c r="B58" s="0"/>
       <c r="C58" s="0"/>
-      <c r="F58" s="42"/>
+      <c r="F58" s="41"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="4" t="s">
@@ -1987,7 +1994,7 @@
       </c>
       <c r="B59" s="0"/>
       <c r="C59" s="0"/>
-      <c r="F59" s="41"/>
+      <c r="F59" s="42"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="4" t="s">
@@ -1995,37 +2002,45 @@
       </c>
       <c r="B60" s="0"/>
       <c r="C60" s="0"/>
-      <c r="F60" s="28"/>
+      <c r="F60" s="41"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="4"/>
+      <c r="A61" s="4" t="s">
+        <v>71</v>
+      </c>
       <c r="B61" s="0"/>
       <c r="C61" s="0"/>
-      <c r="F61" s="5"/>
-    </row>
-    <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="4" t="s">
-        <v>71</v>
-      </c>
+      <c r="F61" s="28"/>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="4"/>
       <c r="B62" s="0"/>
       <c r="C62" s="0"/>
-      <c r="E62" s="43"/>
       <c r="F62" s="5"/>
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="B63" s="0"/>
       <c r="C63" s="0"/>
-    </row>
-    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="31" t="s">
-        <v>72</v>
-      </c>
-      <c r="B64" s="5" t="s">
+      <c r="E63" s="43"/>
+      <c r="F63" s="5"/>
+    </row>
+    <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B64" s="0"/>
+      <c r="C64" s="0"/>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="31" t="s">
         <v>73</v>
       </c>
-      <c r="C64" s="5"/>
-    </row>
-    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="B65" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C65" s="5"/>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2049,7 +2064,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
+      <selection pane="bottomLeft" activeCell="C24" activeCellId="1" sqref="E55 C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2320,7 +2335,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B2" s="4" t="n">
         <v>1</v>
@@ -2579,7 +2594,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="31" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B3" s="46" t="n">
         <v>0</v>
@@ -2838,7 +2853,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="31" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B4" s="46" t="n">
         <v>0</v>
@@ -3097,7 +3112,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="31" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B5" s="4" t="n">
         <v>512</v>
@@ -3356,7 +3371,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="47" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B6" s="46" t="n">
         <v>90</v>
@@ -3615,7 +3630,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="48" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B7" s="46" t="n">
         <v>9</v>
@@ -3874,7 +3889,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="31" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B8" s="4" t="n">
         <v>1500</v>
@@ -4133,7 +4148,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>250</v>
@@ -4392,7 +4407,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B10" s="49"/>
       <c r="C10" s="49"/>
@@ -4647,7 +4662,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="38" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B11" s="0"/>
       <c r="C11" s="0"/>
@@ -4902,7 +4917,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B12" s="50"/>
       <c r="C12" s="0"/>
@@ -5157,7 +5172,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>50</v>
@@ -5416,7 +5431,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="51" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B14" s="52" t="n">
         <v>-1</v>
@@ -5675,7 +5690,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="53" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B15" s="0"/>
       <c r="C15" s="54"/>
@@ -5930,7 +5945,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="53" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B16" s="0"/>
       <c r="C16" s="54"/>
@@ -6185,7 +6200,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="55" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B17" s="56"/>
       <c r="C17" s="57"/>
@@ -6440,7 +6455,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B18" s="0"/>
       <c r="C18" s="0"/>
@@ -6948,7 +6963,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B20" s="50"/>
       <c r="C20" s="58"/>
@@ -7203,7 +7218,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B21" s="50"/>
       <c r="C21" s="58"/>
@@ -7458,7 +7473,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B22" s="0"/>
       <c r="C22" s="0"/>
@@ -7713,7 +7728,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B23" s="0"/>
       <c r="C23" s="0"/>
@@ -7968,7 +7983,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B24" s="0" t="n">
         <f aca="false">B9*0.9</f>
@@ -8482,7 +8497,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B26" s="5" t="n">
         <v>15</v>
@@ -8741,7 +8756,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B27" s="5" t="n">
         <v>2</v>
@@ -9005,7 +9020,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>512</v>
@@ -9016,7 +9031,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>512</v>
@@ -9027,7 +9042,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>1</v>
@@ -9038,7 +9053,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>1</v>
@@ -9049,7 +9064,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B33" s="0"/>
       <c r="C33" s="0"/>
@@ -9061,7 +9076,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B35" s="59" t="n">
         <v>65.1186367</v>
@@ -9072,7 +9087,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B36" s="59" t="n">
         <v>-147.432975</v>
@@ -9088,7 +9103,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B38" s="4" t="n">
         <v>77.51</v>
@@ -9099,7 +9114,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="4" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B39" s="4" t="n">
         <v>19.92</v>
@@ -9110,24 +9125,24 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9137,7 +9152,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="44" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="B43" s="60" t="n">
         <f aca="false">(0.0016)^2</f>
@@ -9150,7 +9165,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="44" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B44" s="44" t="n">
         <v>1</v>
@@ -9161,7 +9176,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="44" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B45" s="44" t="n">
         <v>1</v>
@@ -9190,10 +9205,10 @@
   </sheetPr>
   <dimension ref="A1:JR18"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="J2" activeCellId="0" sqref="J2"/>
+      <selection pane="bottomLeft" activeCell="J2" activeCellId="1" sqref="E55 J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -9498,9 +9513,9 @@
       <c r="JQ1" s="61"/>
       <c r="JR1" s="61"/>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B2" s="63" t="n">
         <v>0</v>
@@ -9529,7 +9544,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>-10.25</v>
@@ -9558,17 +9573,17 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B6" s="4" t="n">
         <v>0.1</v>
@@ -9597,7 +9612,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>1</v>
@@ -9626,65 +9641,65 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="I8" s="4" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="I9" s="4" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>5000</v>
@@ -9713,7 +9728,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B12" s="49" t="n">
         <v>2800000000000</v>
@@ -9742,7 +9757,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>0.375</v>
@@ -9771,7 +9786,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>0.8</v>
@@ -9800,7 +9815,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>2.5</v>
@@ -9829,7 +9844,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>3.5</v>
@@ -9858,7 +9873,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>10000</v>
@@ -9887,7 +9902,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>0.2</v>

</xml_diff>